<commit_message>
Update: id do cliente
</commit_message>
<xml_diff>
--- a/Excel/vendedor_vinil.xlsx
+++ b/Excel/vendedor_vinil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Documents\GitHub\data_warehouse\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21D624D-6572-4F80-9DFA-F30735A12160}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB3C7C-D147-44E2-96FC-D5A48AA6CAA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{6BA8691E-287A-47E0-AAB8-62188D4FB6C9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="91">
   <si>
     <t>nr faixas</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>id cliente</t>
   </si>
 </sst>
 </file>
@@ -667,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C8167B-0E28-4DAE-AF3E-F64A90DC4B9F}">
   <dimension ref="B3:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3:Y8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,10 +682,12 @@
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
     <col min="24" max="24" width="13.42578125" customWidth="1"/>
     <col min="25" max="25" width="16.28515625" customWidth="1"/>
   </cols>
@@ -722,21 +727,24 @@
         <v>17</v>
       </c>
       <c r="M3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>87</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>26</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -774,22 +782,25 @@
       <c r="L4" s="3">
         <v>43427</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>68</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>66</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>36</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>916759846</v>
       </c>
       <c r="X4" s="3"/>
@@ -829,22 +840,25 @@
       <c r="L5" s="3">
         <v>43427</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
         <v>31</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>68</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>36</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>916759846</v>
       </c>
       <c r="X5" s="3"/>
@@ -884,22 +898,25 @@
       <c r="L6" s="3">
         <v>43431</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>68</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>66</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>917543054</v>
       </c>
       <c r="X6" s="3"/>
@@ -939,22 +956,25 @@
       <c r="L7" s="3">
         <v>43431</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
         <v>37</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>69</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>66</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>36</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>919191919</v>
       </c>
       <c r="X7" s="3"/>
@@ -994,22 +1014,25 @@
       <c r="L8" s="3">
         <v>43431</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8" t="s">
         <v>32</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>69</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>66</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>36</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>917768954</v>
       </c>
       <c r="X8" s="3"/>
@@ -1049,22 +1072,25 @@
       <c r="L9" s="3">
         <v>43432</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
         <v>37</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>69</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>66</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>36</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>919191919</v>
       </c>
     </row>
@@ -1103,22 +1129,25 @@
       <c r="L10" s="3">
         <v>43432</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
         <v>30</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>70</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>66</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>27</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>916236123</v>
       </c>
     </row>
@@ -1157,22 +1186,25 @@
       <c r="L11" s="3">
         <v>43434</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11" t="s">
         <v>39</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>71</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>67</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>40</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>36</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>924782938</v>
       </c>
     </row>
@@ -1211,22 +1243,25 @@
       <c r="L12" s="3">
         <v>43435</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12" t="s">
         <v>56</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>70</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>66</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>36</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>916734831</v>
       </c>
     </row>
@@ -1265,22 +1300,25 @@
       <c r="L13" s="3">
         <v>43436</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13">
+        <v>8</v>
+      </c>
+      <c r="N13" t="s">
         <v>58</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>72</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>66</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>54</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>36</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>913075028</v>
       </c>
     </row>
@@ -1319,22 +1357,25 @@
       <c r="L14" s="3">
         <v>43472</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14">
+        <v>9</v>
+      </c>
+      <c r="N14" t="s">
         <v>34</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>73</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>66</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>36</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>923567491</v>
       </c>
     </row>
@@ -1373,22 +1414,25 @@
       <c r="L15" s="3">
         <v>43472</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>74</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>66</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>55</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>36</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>916734290</v>
       </c>
     </row>
@@ -1427,26 +1471,29 @@
       <c r="L16" s="3">
         <v>43474</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16">
+        <v>11</v>
+      </c>
+      <c r="N16" t="s">
         <v>33</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>75</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>66</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>52</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>36</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>923475621</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1481,26 +1528,29 @@
       <c r="L17" s="3">
         <v>43476</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17" t="s">
         <v>30</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>70</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>66</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>44</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>27</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>916236123</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1535,26 +1585,29 @@
       <c r="L18" s="3">
         <v>43476</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
         <v>30</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>70</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>66</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>44</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>27</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>916236123</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1589,29 +1642,32 @@
       <c r="L19" s="3">
         <v>43477</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19" t="s">
         <v>32</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>69</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>66</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>41</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>36</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>917768954</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="E20" s="4"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P22" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Carregamento da Pre Dimensao concluida
</commit_message>
<xml_diff>
--- a/Excel/vendedor_vinil.xlsx
+++ b/Excel/vendedor_vinil.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Documents\GitHub\data_warehouse\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\GitHub\data_warehouse\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB3C7C-D147-44E2-96FC-D5A48AA6CAA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EB88A-92B6-4FF2-A4FA-9DE34C91D2D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{6BA8691E-287A-47E0-AAB8-62188D4FB6C9}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>duracao</t>
   </si>
   <si>
-    <t>preco compra</t>
-  </si>
-  <si>
     <t>Babel</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Rock progressivo, Rock experimental</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>The Darkside of the Moon</t>
   </si>
   <si>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t>id cliente</t>
+  </si>
+  <si>
+    <t>compra_preco</t>
+  </si>
+  <si>
+    <t>data_compra</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
   <dimension ref="B3:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,10 +694,10 @@
   <sheetData>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -721,31 +721,31 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
         <v>24</v>
       </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
@@ -753,25 +753,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4">
         <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J4">
         <v>44.99</v>
@@ -786,19 +786,19 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S4">
         <v>916759846</v>
@@ -811,25 +811,25 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5">
         <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5">
         <v>30.49</v>
@@ -844,19 +844,19 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S5">
         <v>916759846</v>
@@ -869,25 +869,25 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F6">
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6">
         <v>45.49</v>
@@ -902,19 +902,19 @@
         <v>2</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S6">
         <v>917543054</v>
@@ -927,25 +927,25 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7">
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <v>14.9</v>
@@ -960,19 +960,19 @@
         <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S7">
         <v>919191919</v>
@@ -985,25 +985,25 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8">
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J8">
         <v>23.99</v>
@@ -1018,19 +1018,19 @@
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S8">
         <v>917768954</v>
@@ -1043,25 +1043,25 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9">
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J9">
         <v>30.49</v>
@@ -1076,19 +1076,19 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S9">
         <v>919191919</v>
@@ -1100,25 +1100,25 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F10">
         <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
         <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>15</v>
       </c>
       <c r="J10">
         <v>99.99</v>
@@ -1133,19 +1133,19 @@
         <v>5</v>
       </c>
       <c r="N10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S10">
         <v>916236123</v>
@@ -1157,25 +1157,25 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11">
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11">
         <v>14.9</v>
@@ -1190,19 +1190,19 @@
         <v>6</v>
       </c>
       <c r="N11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S11">
         <v>924782938</v>
@@ -1214,25 +1214,25 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F12">
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J12">
         <v>34.99</v>
@@ -1247,19 +1247,19 @@
         <v>7</v>
       </c>
       <c r="N12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S12">
         <v>916734831</v>
@@ -1271,25 +1271,25 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J13">
         <v>45.49</v>
@@ -1304,19 +1304,19 @@
         <v>8</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S13">
         <v>913075028</v>
@@ -1328,25 +1328,25 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14">
         <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J14">
         <v>44.99</v>
@@ -1361,19 +1361,19 @@
         <v>9</v>
       </c>
       <c r="N14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>71</v>
+      </c>
+      <c r="P14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R14" t="s">
         <v>34</v>
-      </c>
-      <c r="O14" t="s">
-        <v>73</v>
-      </c>
-      <c r="P14" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>51</v>
-      </c>
-      <c r="R14" t="s">
-        <v>36</v>
       </c>
       <c r="S14">
         <v>923567491</v>
@@ -1385,25 +1385,25 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15">
         <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F15">
         <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J15">
         <v>42.49</v>
@@ -1418,19 +1418,19 @@
         <v>10</v>
       </c>
       <c r="N15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S15">
         <v>916734290</v>
@@ -1442,25 +1442,25 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16">
         <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
         <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
       </c>
       <c r="J16">
         <v>99.99</v>
@@ -1475,19 +1475,19 @@
         <v>11</v>
       </c>
       <c r="N16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S16">
         <v>923475621</v>
@@ -1499,25 +1499,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F17">
         <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
         <v>21</v>
-      </c>
-      <c r="I17" t="s">
-        <v>23</v>
       </c>
       <c r="J17">
         <v>25.99</v>
@@ -1532,19 +1532,19 @@
         <v>5</v>
       </c>
       <c r="N17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S17">
         <v>916236123</v>
@@ -1556,25 +1556,25 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18">
         <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18">
         <v>14.9</v>
@@ -1589,19 +1589,19 @@
         <v>5</v>
       </c>
       <c r="N18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S18">
         <v>916236123</v>
@@ -1613,25 +1613,25 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F19">
         <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J19">
         <v>34.99</v>
@@ -1646,19 +1646,19 @@
         <v>4</v>
       </c>
       <c r="N19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S19">
         <v>917768954</v>

</xml_diff>